<commit_message>
I combine the delete,edit,find cases in one called manage cases
</commit_message>
<xml_diff>
--- a/uploads/cases.xlsx
+++ b/uploads/cases.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P11"/>
+  <dimension ref="A1:P21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -517,7 +517,7 @@
         <v>Fine ₱5,000</v>
       </c>
       <c r="P2" t="str">
-        <v>/uploads/index_cards/indexcard-1768197910097-55613769.png</v>
+        <v>/uploads/index_cards/indexcard-1768207654861-25492876.png</v>
       </c>
     </row>
     <row r="3">
@@ -949,9 +949,491 @@
         <v>Mischief-2025</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12">
+        <v>36</v>
+      </c>
+      <c r="B12" t="str">
+        <v>NPS-III-2025-065</v>
+      </c>
+      <c r="C12" t="str">
+        <v>Invalid Date</v>
+      </c>
+      <c r="D12" t="str">
+        <v>Rainer Antiola</v>
+      </c>
+      <c r="E12" t="str">
+        <v>Justin Merina</v>
+      </c>
+      <c r="F12" t="str">
+        <v>78 Del Pilar St., Manila</v>
+      </c>
+      <c r="G12" t="str">
+        <v>Physical Injuries</v>
+      </c>
+      <c r="I12" t="str">
+        <v>Invalid Date</v>
+      </c>
+      <c r="J12" t="str">
+        <v>Atty. P. Navarro</v>
+      </c>
+      <c r="K12" t="str">
+        <v>25-1062</v>
+      </c>
+      <c r="L12" t="str">
+        <v>MTC Br. 4, Manila</v>
+      </c>
+      <c r="M12" t="str">
+        <v>Invalid Date</v>
+      </c>
+      <c r="N12" t="str">
+        <v>Information filed</v>
+      </c>
+      <c r="O12" t="str">
+        <v>Community service</v>
+      </c>
+      <c r="P12" t="str">
+        <v>Injuries-2025</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
+        <v>37</v>
+      </c>
+      <c r="B13" t="str">
+        <v>NPS-III-2025-099</v>
+      </c>
+      <c r="C13" t="str">
+        <v>Invalid Date</v>
+      </c>
+      <c r="D13" t="str">
+        <v>Kershua</v>
+      </c>
+      <c r="E13" t="str">
+        <v>Jeffy</v>
+      </c>
+      <c r="F13" t="str">
+        <v>Sitio Mabuhay, Cebu City</v>
+      </c>
+      <c r="G13" t="str">
+        <v>Illegal Possession of Firearms</v>
+      </c>
+      <c r="I13" t="str">
+        <v>Invalid Date</v>
+      </c>
+      <c r="J13" t="str">
+        <v>Atty. S. Morales</v>
+      </c>
+      <c r="K13" t="str">
+        <v>25-1070</v>
+      </c>
+      <c r="L13" t="str">
+        <v>RTC Br. 12, Cebu</v>
+      </c>
+      <c r="M13" t="str">
+        <v>Invalid Date</v>
+      </c>
+      <c r="N13" t="str">
+        <v>Information filed</v>
+      </c>
+      <c r="O13" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="P13" t="str">
+        <v>Firearms-2025</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14">
+        <v>38</v>
+      </c>
+      <c r="B14" t="str">
+        <v>NPS-III-2025-088</v>
+      </c>
+      <c r="C14" t="str">
+        <v>Invalid Date</v>
+      </c>
+      <c r="D14" t="str">
+        <v>Miguel Ohara</v>
+      </c>
+      <c r="E14" t="str">
+        <v>Peter Parker</v>
+      </c>
+      <c r="F14" t="str">
+        <v>210 Luna St., Makati City</v>
+      </c>
+      <c r="G14" t="str">
+        <v>Cyber Libel</v>
+      </c>
+      <c r="I14" t="str">
+        <v>Invalid Date</v>
+      </c>
+      <c r="J14" t="str">
+        <v>Atty. E. Flores</v>
+      </c>
+      <c r="K14" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="L14" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="M14" t="str">
+        <v>Invalid Date</v>
+      </c>
+      <c r="N14" t="str">
+        <v>Pending</v>
+      </c>
+      <c r="O14" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="P14" t="str">
+        <v>Cybercrime-2025</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15">
+        <v>39</v>
+      </c>
+      <c r="B15" t="str">
+        <v>NPS-III-2025-067</v>
+      </c>
+      <c r="C15" t="str">
+        <v>Invalid Date</v>
+      </c>
+      <c r="D15" t="str">
+        <v>Michael jackson</v>
+      </c>
+      <c r="E15" t="str">
+        <v>Justin Bieber</v>
+      </c>
+      <c r="F15" t="str">
+        <v>56 Chino Roces Ave., Makati</v>
+      </c>
+      <c r="G15" t="str">
+        <v>Bouncing Checks (BP 22)</v>
+      </c>
+      <c r="I15" t="str">
+        <v>Invalid Date</v>
+      </c>
+      <c r="J15" t="str">
+        <v>Atty. M. Gomez</v>
+      </c>
+      <c r="K15" t="str">
+        <v>25-1081</v>
+      </c>
+      <c r="L15" t="str">
+        <v>MTC Br. 6, Makati</v>
+      </c>
+      <c r="M15" t="str">
+        <v>Invalid Date</v>
+      </c>
+      <c r="N15" t="str">
+        <v>Information filed</v>
+      </c>
+      <c r="O15" t="str">
+        <v>Fine ₱20,000</v>
+      </c>
+      <c r="P15" t="str">
+        <v>BP22-2025</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16">
+        <v>40</v>
+      </c>
+      <c r="B16" t="str">
+        <v>No: NPS-III-2025-030</v>
+      </c>
+      <c r="C16" t="str">
+        <v>Invalid Date</v>
+      </c>
+      <c r="D16" t="str">
+        <v>Obiwan Kenobi</v>
+      </c>
+      <c r="E16" t="str">
+        <v>Luke  Skywalker</v>
+      </c>
+      <c r="F16" t="str">
+        <v>Barangay Sta. Cruz, Manila</v>
+      </c>
+      <c r="G16" t="str">
+        <v>Murder</v>
+      </c>
+      <c r="I16" t="str">
+        <v>Invalid Date</v>
+      </c>
+      <c r="J16" t="str">
+        <v>Atty. J. Cruz</v>
+      </c>
+      <c r="K16" t="str">
+        <v>25-1090</v>
+      </c>
+      <c r="L16" t="str">
+        <v>RTC Br. 51, Manila</v>
+      </c>
+      <c r="M16" t="str">
+        <v>Invalid Date</v>
+      </c>
+      <c r="N16" t="str">
+        <v>Information filed</v>
+      </c>
+      <c r="O16" t="str">
+        <v>Death Penalty</v>
+      </c>
+      <c r="P16" t="str">
+        <v>QTheft-2025</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17">
+        <v>41</v>
+      </c>
+      <c r="B17" t="str">
+        <v>NPS-III-2025-047</v>
+      </c>
+      <c r="C17" t="str">
+        <v>Invalid Date</v>
+      </c>
+      <c r="D17" t="str">
+        <v>Arvin Antiola</v>
+      </c>
+      <c r="E17" t="str">
+        <v>Harry Potter</v>
+      </c>
+      <c r="F17" t="str">
+        <v>89 Bonifacio St., Caloocan City</v>
+      </c>
+      <c r="G17" t="str">
+        <v>Malicious Mischief</v>
+      </c>
+      <c r="I17" t="str">
+        <v>Invalid Date</v>
+      </c>
+      <c r="J17" t="str">
+        <v>Atty. L. Ramirez</v>
+      </c>
+      <c r="K17" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="L17" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="M17" t="str">
+        <v>Invalid Date</v>
+      </c>
+      <c r="N17" t="str">
+        <v>Case dismissed</v>
+      </c>
+      <c r="O17" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="P17" t="str">
+        <v>Mischief-2026</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18">
+        <v>42</v>
+      </c>
+      <c r="B18" t="str">
+        <v>NPS-III-2025-001</v>
+      </c>
+      <c r="C18" t="str">
+        <v>Invalid Date</v>
+      </c>
+      <c r="D18" t="str">
+        <v>Jakerax</v>
+      </c>
+      <c r="E18" t="str">
+        <v>Kian Arcayan</v>
+      </c>
+      <c r="F18" t="str">
+        <v>123 Mabini St., Quezon City</v>
+      </c>
+      <c r="G18" t="str">
+        <v>Theft</v>
+      </c>
+      <c r="H18" t="str">
+        <v>Invalid Date</v>
+      </c>
+      <c r="I18" t="str">
+        <v>Invalid Date</v>
+      </c>
+      <c r="J18" t="str">
+        <v>Atty. M. Bullanday</v>
+      </c>
+      <c r="K18" t="str">
+        <v>25-1046</v>
+      </c>
+      <c r="L18" t="str">
+        <v>MTC Br. 2, QC</v>
+      </c>
+      <c r="M18" t="str">
+        <v>Invalid Date</v>
+      </c>
+      <c r="N18" t="str">
+        <v>Information filed</v>
+      </c>
+      <c r="O18" t="str">
+        <v>Fine 1 million</v>
+      </c>
+      <c r="P18" t="str">
+        <v>Theft-2025</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19">
+        <v>43</v>
+      </c>
+      <c r="B19" t="str">
+        <v>NPS-III-2025-031</v>
+      </c>
+      <c r="C19" t="str">
+        <v>Invalid Date</v>
+      </c>
+      <c r="D19" t="str">
+        <v>US Government</v>
+      </c>
+      <c r="E19" t="str">
+        <v>Arvin Birada</v>
+      </c>
+      <c r="F19" t="str">
+        <v>Barangay San Isidro of United States</v>
+      </c>
+      <c r="G19" t="str">
+        <v>Violation of RA 9165</v>
+      </c>
+      <c r="H19" t="str">
+        <v>Invalid Date</v>
+      </c>
+      <c r="I19" t="str">
+        <v>Invalid Date</v>
+      </c>
+      <c r="J19" t="str">
+        <v>Atty. L. Anrcayan</v>
+      </c>
+      <c r="K19" t="str">
+        <v>25-1050</v>
+      </c>
+      <c r="L19" t="str">
+        <v>RTC Br. 88, QC</v>
+      </c>
+      <c r="M19" t="str">
+        <v>Invalid Date</v>
+      </c>
+      <c r="N19" t="str">
+        <v>Information filed</v>
+      </c>
+      <c r="O19" t="str">
+        <v>Death Penalty</v>
+      </c>
+      <c r="P19" t="str">
+        <v>Drugs-2025</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20">
+        <v>44</v>
+      </c>
+      <c r="B20" t="str">
+        <v>NPS-III-2025-000</v>
+      </c>
+      <c r="C20" t="str">
+        <v>Invalid Date</v>
+      </c>
+      <c r="D20" t="str">
+        <v>KIan Perez</v>
+      </c>
+      <c r="E20" t="str">
+        <v>Diddy</v>
+      </c>
+      <c r="F20" t="str">
+        <v>45 Rizal Ave., Manila</v>
+      </c>
+      <c r="G20" t="str">
+        <v>Rape</v>
+      </c>
+      <c r="H20" t="str">
+        <v>Invalid Date</v>
+      </c>
+      <c r="I20" t="str">
+        <v>Invalid Date</v>
+      </c>
+      <c r="J20" t="str">
+        <v>Atty. M. Galamiton</v>
+      </c>
+      <c r="K20" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="L20" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="M20" t="str">
+        <v>Invalid Date</v>
+      </c>
+      <c r="N20" t="str">
+        <v>Case dismissed</v>
+      </c>
+      <c r="O20" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="P20" t="str">
+        <v>Estafa-2025</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21">
+        <v>45</v>
+      </c>
+      <c r="B21" t="str">
+        <v>NPS-III-2025-009</v>
+      </c>
+      <c r="C21" t="str">
+        <v>Invalid Date</v>
+      </c>
+      <c r="D21" t="str">
+        <v>RIck</v>
+      </c>
+      <c r="E21" t="str">
+        <v>Coral</v>
+      </c>
+      <c r="F21" t="str">
+        <v>Purok 3, Barangay Malinis, Laguna</v>
+      </c>
+      <c r="G21" t="str">
+        <v>Grave Threats</v>
+      </c>
+      <c r="H21" t="str">
+        <v>Invalid Date</v>
+      </c>
+      <c r="I21" t="str">
+        <v>Invalid Date</v>
+      </c>
+      <c r="J21" t="str">
+        <v>Atty. R. Bullanday</v>
+      </c>
+      <c r="K21" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="L21" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="M21" t="str">
+        <v>Invalid Date</v>
+      </c>
+      <c r="N21" t="str">
+        <v>Case dismissed</v>
+      </c>
+      <c r="O21" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="P21" t="str">
+        <v>Threats-2025</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:P11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:P21"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add edit button and shield icon for user role management
</commit_message>
<xml_diff>
--- a/uploads/cases.xlsx
+++ b/uploads/cases.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P10"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -472,46 +472,49 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B2" t="str">
-        <v>DKT-2024-003</v>
+        <v>2026-123</v>
       </c>
       <c r="C2" t="str">
-        <v>2024-03-07</v>
+        <v>Invalid Date</v>
       </c>
       <c r="D2" t="str">
-        <v>BIR</v>
+        <v>judegs</v>
       </c>
       <c r="E2" t="str">
-        <v>ABC Company Inc</v>
+        <v>elaine</v>
       </c>
       <c r="F2" t="str">
-        <v>San Isidro</v>
+        <v>loboc</v>
       </c>
       <c r="G2" t="str">
-        <v>Tax Evasion</v>
+        <v>Physical Injury</v>
       </c>
       <c r="H2" t="str">
-        <v>2026-01-26</v>
+        <v>Invalid Date</v>
+      </c>
+      <c r="I2" t="str">
+        <v>2026-01-23</v>
       </c>
       <c r="J2" t="str">
-        <v>Prosecutor Lopez</v>
+        <v>Atty. ramosola</v>
       </c>
       <c r="K2" t="str">
-        <v>CRIM-2024-003</v>
+        <v>CCN-003</v>
       </c>
       <c r="L2" t="str">
-        <v>Branch 1</v>
+        <v>Branch 3</v>
       </c>
       <c r="M2" t="str">
-        <v>2024-04-02</v>
+        <v>2026-01-16</v>
       </c>
       <c r="N2" t="str">
-        <v>dismissed</v>
+        <v>Pending</v>
       </c>
       <c r="O2" t="str">
-        <v>Pending</v>
+        <v>100k</v>
       </c>
       <c r="P2" t="str">
         <v>N/A</v>
@@ -519,49 +522,49 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B3" t="str">
-        <v>182938123</v>
+        <v>2026-0654</v>
       </c>
       <c r="C3" t="str">
-        <v>2026-01-04</v>
+        <v>Invalid Date</v>
       </c>
       <c r="D3" t="str">
-        <v>pakyaw</v>
+        <v>huan</v>
       </c>
       <c r="E3" t="str">
-        <v>samsung</v>
+        <v>jigss</v>
       </c>
       <c r="F3" t="str">
-        <v>Loboc</v>
+        <v>loon</v>
       </c>
       <c r="G3" t="str">
-        <v>robbery</v>
+        <v>grave threat</v>
       </c>
       <c r="H3" t="str">
-        <v>2026-01-15</v>
+        <v>Invalid Date</v>
       </c>
       <c r="I3" t="str">
-        <v>2026-01-05</v>
+        <v>Invalid Date</v>
       </c>
       <c r="J3" t="str">
-        <v>james</v>
+        <v>Atty. ramosola</v>
       </c>
       <c r="K3" t="str">
-        <v>Reppublic Act 2104</v>
+        <v>CCN-004</v>
       </c>
       <c r="L3" t="str">
-        <v>Tagbi</v>
+        <v>Branch 5</v>
       </c>
       <c r="M3" t="str">
-        <v>2026-01-06</v>
+        <v>2026-02-16</v>
       </c>
       <c r="N3" t="str">
-        <v>convicted</v>
+        <v>Dismissed</v>
       </c>
       <c r="O3" t="str">
-        <v>14k</v>
+        <v/>
       </c>
       <c r="P3" t="str">
         <v>N/A</v>
@@ -569,99 +572,99 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B4" t="str">
-        <v>65435232</v>
+        <v>2026-112</v>
       </c>
       <c r="C4" t="str">
-        <v>2026-01-27</v>
+        <v>Invalid Date</v>
       </c>
       <c r="D4" t="str">
-        <v>samsup</v>
+        <v>sanee</v>
       </c>
       <c r="E4" t="str">
-        <v>huawei</v>
+        <v>sanity</v>
       </c>
       <c r="F4" t="str">
-        <v>Taloto</v>
+        <v>sagbay</v>
       </c>
       <c r="G4" t="str">
-        <v>raped</v>
+        <v>stabbed</v>
       </c>
       <c r="H4" t="str">
         <v>2026-01-22</v>
       </c>
       <c r="I4" t="str">
-        <v>2026-01-11</v>
+        <v>2026-01-27</v>
       </c>
       <c r="J4" t="str">
-        <v>Atty. Doroy</v>
+        <v>atty.guardarama</v>
       </c>
       <c r="K4" t="str">
         <v>N/A</v>
       </c>
       <c r="L4" t="str">
-        <v>Capitol</v>
+        <v>Branch 2</v>
       </c>
       <c r="M4" t="str">
-        <v>2026-01-20</v>
+        <v>2026-01-29</v>
       </c>
       <c r="N4" t="str">
-        <v>pending</v>
+        <v>Convicted</v>
       </c>
       <c r="O4" t="str">
-        <v>15k</v>
+        <v>200k</v>
       </c>
       <c r="P4" t="str">
-        <v>N/A</v>
+        <v>/uploads/index_cards/indexcard-1768809005939-642131609.png</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B5" t="str">
-        <v>13242141</v>
+        <v>2026-009</v>
       </c>
       <c r="C5" t="str">
         <v>Invalid Date</v>
       </c>
       <c r="D5" t="str">
-        <v>manny</v>
+        <v>koka</v>
       </c>
       <c r="E5" t="str">
-        <v>clifford</v>
+        <v>langasa</v>
       </c>
       <c r="F5" t="str">
-        <v>San isidro</v>
+        <v>tubigon</v>
       </c>
       <c r="G5" t="str">
-        <v>theft</v>
+        <v>raper</v>
       </c>
       <c r="H5" t="str">
         <v>Invalid Date</v>
       </c>
       <c r="I5" t="str">
-        <v>2026-01-08</v>
+        <v>Invalid Date</v>
       </c>
       <c r="J5" t="str">
-        <v>james</v>
+        <v>Atty. ramosola</v>
       </c>
       <c r="K5" t="str">
-        <v>Reppublic Act 2104</v>
+        <v>CCN-009</v>
       </c>
       <c r="L5" t="str">
-        <v>Tagbi</v>
+        <v>Branch 4</v>
       </c>
       <c r="M5" t="str">
-        <v>2026-01-09</v>
+        <v>2026-07-17</v>
       </c>
       <c r="N5" t="str">
-        <v>pending</v>
+        <v>Pending</v>
       </c>
       <c r="O5" t="str">
-        <v>14k</v>
+        <v/>
       </c>
       <c r="P5" t="str">
         <v>N/A</v>
@@ -669,49 +672,49 @@
     </row>
     <row r="6">
       <c r="A6">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B6" t="str">
-        <v>76543232</v>
+        <v>2026-010</v>
       </c>
       <c r="C6" t="str">
         <v>Invalid Date</v>
       </c>
       <c r="D6" t="str">
-        <v>namiiiii</v>
+        <v>shagu</v>
       </c>
       <c r="E6" t="str">
-        <v>chriss</v>
+        <v>marinate</v>
       </c>
       <c r="F6" t="str">
-        <v>buol</v>
+        <v>loboc</v>
       </c>
       <c r="G6" t="str">
-        <v>raped</v>
+        <v>muder</v>
       </c>
       <c r="H6" t="str">
         <v>Invalid Date</v>
       </c>
       <c r="I6" t="str">
-        <v>2026-01-13</v>
+        <v>Invalid Date</v>
       </c>
       <c r="J6" t="str">
-        <v>Atty. Doroy</v>
+        <v>Atty. ramosola</v>
       </c>
       <c r="K6" t="str">
-        <v>N/A</v>
+        <v>CCN-010</v>
       </c>
       <c r="L6" t="str">
-        <v>Capitol</v>
+        <v>Branch 1</v>
       </c>
       <c r="M6" t="str">
-        <v>2026-01-22</v>
+        <v>2026-08-17</v>
       </c>
       <c r="N6" t="str">
-        <v>pending</v>
+        <v>Convicted</v>
       </c>
       <c r="O6" t="str">
-        <v>15k</v>
+        <v/>
       </c>
       <c r="P6" t="str">
         <v>N/A</v>
@@ -719,207 +722,57 @@
     </row>
     <row r="7">
       <c r="A7">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B7" t="str">
-        <v>235845323</v>
+        <v>2026-011</v>
       </c>
       <c r="C7" t="str">
-        <v>2026-02-06</v>
+        <v>Invalid Date</v>
       </c>
       <c r="D7" t="str">
-        <v>jek2</v>
+        <v>shaggyy</v>
       </c>
       <c r="E7" t="str">
-        <v>zuma</v>
+        <v>silasa</v>
       </c>
       <c r="F7" t="str">
-        <v>manalo</v>
+        <v>loboc</v>
       </c>
       <c r="G7" t="str">
-        <v>grave threat</v>
+        <v>homicide</v>
       </c>
       <c r="H7" t="str">
-        <v>2026-01-29</v>
+        <v>Invalid Date</v>
       </c>
       <c r="I7" t="str">
         <v>Invalid Date</v>
       </c>
       <c r="J7" t="str">
-        <v>Atty .spiderman</v>
+        <v>Atty. ramosola</v>
       </c>
       <c r="K7" t="str">
-        <v>N/A</v>
+        <v>CCN-122</v>
       </c>
       <c r="L7" t="str">
-        <v>N/A</v>
+        <v>Branch 3</v>
       </c>
       <c r="M7" t="str">
-        <v>2026-01-21</v>
+        <v>2026-09-15</v>
       </c>
       <c r="N7" t="str">
-        <v>Dismissed</v>
+        <v/>
       </c>
       <c r="O7" t="str">
-        <v>23k</v>
+        <v/>
       </c>
       <c r="P7" t="str">
-        <v>N/A</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8">
-        <v>11</v>
-      </c>
-      <c r="B8" t="str">
-        <v>16234</v>
-      </c>
-      <c r="C8" t="str">
-        <v>2026-01-07</v>
-      </c>
-      <c r="D8" t="str">
-        <v>roxanne</v>
-      </c>
-      <c r="E8" t="str">
-        <v>kristtian</v>
-      </c>
-      <c r="F8" t="str">
-        <v>cabanugan</v>
-      </c>
-      <c r="G8" t="str">
-        <v>robbery</v>
-      </c>
-      <c r="H8" t="str">
-        <v>Invalid Date</v>
-      </c>
-      <c r="I8" t="str">
-        <v>2026-01-08</v>
-      </c>
-      <c r="J8" t="str">
-        <v>james</v>
-      </c>
-      <c r="K8" t="str">
-        <v>Reppublic Act 2104</v>
-      </c>
-      <c r="L8" t="str">
-        <v>Tagbi</v>
-      </c>
-      <c r="M8" t="str">
-        <v>2026-01-09</v>
-      </c>
-      <c r="N8" t="str">
-        <v>pending</v>
-      </c>
-      <c r="O8" t="str">
-        <v>14k</v>
-      </c>
-      <c r="P8" t="str">
-        <v>N/A</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9">
-        <v>12</v>
-      </c>
-      <c r="B9" t="str">
-        <v>72341</v>
-      </c>
-      <c r="C9" t="str">
-        <v>2026-01-07</v>
-      </c>
-      <c r="D9" t="str">
-        <v>marcilene</v>
-      </c>
-      <c r="E9" t="str">
-        <v>shielouu</v>
-      </c>
-      <c r="F9" t="str">
-        <v>cansage norte</v>
-      </c>
-      <c r="G9" t="str">
-        <v>grave threat</v>
-      </c>
-      <c r="H9" t="str">
-        <v>Invalid Date</v>
-      </c>
-      <c r="I9" t="str">
-        <v>2026-01-30</v>
-      </c>
-      <c r="J9" t="str">
-        <v>Atty. Superman</v>
-      </c>
-      <c r="K9" t="str">
-        <v>N/A</v>
-      </c>
-      <c r="L9" t="str">
-        <v>tagbi</v>
-      </c>
-      <c r="M9" t="str">
-        <v>2026-01-29</v>
-      </c>
-      <c r="N9" t="str">
-        <v>Convicted</v>
-      </c>
-      <c r="O9" t="str">
-        <v>100k</v>
-      </c>
-      <c r="P9" t="str">
-        <v>N/A</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10">
-        <v>13</v>
-      </c>
-      <c r="B10" t="str">
-        <v>115532</v>
-      </c>
-      <c r="C10" t="str">
-        <v>2026-01-29</v>
-      </c>
-      <c r="D10" t="str">
-        <v>mercyyy</v>
-      </c>
-      <c r="E10" t="str">
-        <v>tibinn</v>
-      </c>
-      <c r="F10" t="str">
-        <v>baunos</v>
-      </c>
-      <c r="G10" t="str">
-        <v>raped</v>
-      </c>
-      <c r="H10" t="str">
-        <v>Invalid Date</v>
-      </c>
-      <c r="I10" t="str">
-        <v>2026-01-13</v>
-      </c>
-      <c r="J10" t="str">
-        <v>Atty. Doroy</v>
-      </c>
-      <c r="K10" t="str">
-        <v>N/A</v>
-      </c>
-      <c r="L10" t="str">
-        <v>Capitol</v>
-      </c>
-      <c r="M10" t="str">
-        <v>2026-01-22</v>
-      </c>
-      <c r="N10" t="str">
-        <v>Dismissed</v>
-      </c>
-      <c r="O10" t="str">
-        <v>190k</v>
-      </c>
-      <c r="P10" t="str">
         <v>N/A</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:P10"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:P7"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Implemented a Type Script
</commit_message>
<xml_diff>
--- a/uploads/cases.xlsx
+++ b/uploads/cases.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P8"/>
+  <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -820,9 +820,159 @@
         <v>N/A</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9">
+        <v>14</v>
+      </c>
+      <c r="B9" t="str">
+        <v>3232</v>
+      </c>
+      <c r="C9" t="str">
+        <v>2026-01-07</v>
+      </c>
+      <c r="D9" t="str">
+        <v>keynn</v>
+      </c>
+      <c r="E9" t="str">
+        <v>trekk</v>
+      </c>
+      <c r="F9" t="str">
+        <v>San Isidro</v>
+      </c>
+      <c r="G9" t="str">
+        <v>robbery</v>
+      </c>
+      <c r="H9" t="str">
+        <v>Invalid Date</v>
+      </c>
+      <c r="I9" t="str">
+        <v>2026-01-08</v>
+      </c>
+      <c r="J9" t="str">
+        <v>Atty.batman</v>
+      </c>
+      <c r="K9" t="str">
+        <v>Reppublic Act 2104</v>
+      </c>
+      <c r="L9" t="str">
+        <v>Tagbi</v>
+      </c>
+      <c r="M9" t="str">
+        <v>2026-01-09</v>
+      </c>
+      <c r="N9" t="str">
+        <v>pending</v>
+      </c>
+      <c r="O9" t="str">
+        <v>14k</v>
+      </c>
+      <c r="P9" t="str">
+        <v>N/A</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>15</v>
+      </c>
+      <c r="B10" t="str">
+        <v>245232</v>
+      </c>
+      <c r="C10" t="str">
+        <v>2026-01-07</v>
+      </c>
+      <c r="D10" t="str">
+        <v>koynnn</v>
+      </c>
+      <c r="E10" t="str">
+        <v>kart</v>
+      </c>
+      <c r="F10" t="str">
+        <v xml:space="preserve">Tiptip </v>
+      </c>
+      <c r="G10" t="str">
+        <v>grave threat</v>
+      </c>
+      <c r="H10" t="str">
+        <v>Invalid Date</v>
+      </c>
+      <c r="I10" t="str">
+        <v>2026-01-30</v>
+      </c>
+      <c r="J10" t="str">
+        <v>Atty. Superman</v>
+      </c>
+      <c r="K10" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="L10" t="str">
+        <v>tagbi</v>
+      </c>
+      <c r="M10" t="str">
+        <v>2026-01-29</v>
+      </c>
+      <c r="N10" t="str">
+        <v>terminated</v>
+      </c>
+      <c r="O10" t="str">
+        <v>12k</v>
+      </c>
+      <c r="P10" t="str">
+        <v>N/A</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>16</v>
+      </c>
+      <c r="B11" t="str">
+        <v>4121214</v>
+      </c>
+      <c r="C11" t="str">
+        <v>2026-01-29</v>
+      </c>
+      <c r="D11" t="str">
+        <v>shaaan</v>
+      </c>
+      <c r="E11" t="str">
+        <v>kroel</v>
+      </c>
+      <c r="F11" t="str">
+        <v>Dauis</v>
+      </c>
+      <c r="G11" t="str">
+        <v>raped</v>
+      </c>
+      <c r="H11" t="str">
+        <v>Invalid Date</v>
+      </c>
+      <c r="I11" t="str">
+        <v>2026-01-13</v>
+      </c>
+      <c r="J11" t="str">
+        <v>Atty. Doroy</v>
+      </c>
+      <c r="K11" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="L11" t="str">
+        <v>Capitol</v>
+      </c>
+      <c r="M11" t="str">
+        <v>2026-01-22</v>
+      </c>
+      <c r="N11" t="str">
+        <v>pending</v>
+      </c>
+      <c r="O11" t="str">
+        <v>15k</v>
+      </c>
+      <c r="P11" t="str">
+        <v>N/A</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:P8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:P11"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
More on Frontends Improved
</commit_message>
<xml_diff>
--- a/uploads/cases.xlsx
+++ b/uploads/cases.xlsx
@@ -397,582 +397,454 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P11"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="5.83203125" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" customWidth="1"/>
-    <col min="3" max="3" width="12.83203125" customWidth="1"/>
+    <col min="1" max="1" width="15.83203125" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" customWidth="1"/>
+    <col min="3" max="3" width="20.83203125" customWidth="1"/>
     <col min="4" max="4" width="20.83203125" customWidth="1"/>
-    <col min="5" max="5" width="20.83203125" customWidth="1"/>
-    <col min="6" max="6" width="30.83203125" customWidth="1"/>
-    <col min="7" max="7" width="20.83203125" customWidth="1"/>
-    <col min="8" max="8" width="15.83203125" customWidth="1"/>
-    <col min="9" max="9" width="12.83203125" customWidth="1"/>
-    <col min="10" max="10" width="20.83203125" customWidth="1"/>
-    <col min="11" max="11" width="15.83203125" customWidth="1"/>
-    <col min="12" max="12" width="12.83203125" customWidth="1"/>
+    <col min="5" max="5" width="30.83203125" customWidth="1"/>
+    <col min="6" max="6" width="20.83203125" customWidth="1"/>
+    <col min="7" max="7" width="15.83203125" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" customWidth="1"/>
+    <col min="9" max="9" width="20.83203125" customWidth="1"/>
+    <col min="10" max="10" width="15.83203125" customWidth="1"/>
+    <col min="11" max="11" width="12.83203125" customWidth="1"/>
+    <col min="12" max="12" width="15.83203125" customWidth="1"/>
     <col min="13" max="13" width="15.83203125" customWidth="1"/>
-    <col min="14" max="14" width="15.83203125" customWidth="1"/>
-    <col min="15" max="15" width="12.83203125" customWidth="1"/>
-    <col min="16" max="16" width="50.83203125" customWidth="1"/>
+    <col min="14" max="14" width="12.83203125" customWidth="1"/>
+    <col min="15" max="15" width="50.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>ID</v>
+        <v>Docket No</v>
       </c>
       <c r="B1" t="str">
-        <v>Docket No</v>
+        <v>Date Filed</v>
       </c>
       <c r="C1" t="str">
-        <v>Date Filed</v>
+        <v>Complainant</v>
       </c>
       <c r="D1" t="str">
-        <v>Complainant</v>
+        <v>Respondent</v>
       </c>
       <c r="E1" t="str">
-        <v>Respondent</v>
+        <v>Address of Respondent</v>
       </c>
       <c r="F1" t="str">
-        <v>Address of Respondent</v>
+        <v>Offense</v>
       </c>
       <c r="G1" t="str">
-        <v>Offense</v>
+        <v>Date of Commission</v>
       </c>
       <c r="H1" t="str">
-        <v>Date of Commission</v>
+        <v>Date Resolved</v>
       </c>
       <c r="I1" t="str">
-        <v>Date Resolved</v>
+        <v>Resolving Prosecutor</v>
       </c>
       <c r="J1" t="str">
-        <v>Resolving Prosecutor</v>
+        <v>Criminal Case No</v>
       </c>
       <c r="K1" t="str">
-        <v>Criminal Case No</v>
+        <v>Branch</v>
       </c>
       <c r="L1" t="str">
-        <v>Branch</v>
+        <v>Date Filed in Court</v>
       </c>
       <c r="M1" t="str">
-        <v>Date Filed in Court</v>
+        <v>Remarks Decision</v>
       </c>
       <c r="N1" t="str">
-        <v>Remarks Decision</v>
+        <v>Penalty</v>
       </c>
       <c r="O1" t="str">
-        <v>Penalty</v>
-      </c>
-      <c r="P1" t="str">
         <v>Index Cards</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2">
-        <v>6</v>
+      <c r="A2" t="str">
+        <v>DKT-2024-001</v>
       </c>
       <c r="B2" t="str">
-        <v>65435232</v>
+        <v>2024-01-10</v>
       </c>
       <c r="C2" t="str">
-        <v>2026-01-27</v>
+        <v>PNP Tagbilaran</v>
       </c>
       <c r="D2" t="str">
-        <v>samsup</v>
+        <v>John Doe</v>
       </c>
       <c r="E2" t="str">
-        <v>huawei</v>
+        <v>loon</v>
       </c>
       <c r="F2" t="str">
-        <v>Taloto</v>
+        <v>Theft</v>
       </c>
       <c r="G2" t="str">
-        <v>raped</v>
+        <v>Invalid Date</v>
       </c>
       <c r="H2" t="str">
-        <v>2026-01-22</v>
+        <v>2024-03-15</v>
       </c>
       <c r="I2" t="str">
-        <v>2026-01-11</v>
+        <v>Prosecutor Martinez</v>
       </c>
       <c r="J2" t="str">
-        <v>Atty. Doroy</v>
+        <v>CRIM-2024-001</v>
       </c>
       <c r="K2" t="str">
-        <v>N/A</v>
+        <v>Branch 1</v>
       </c>
       <c r="L2" t="str">
-        <v>Capitol</v>
+        <v>2024-02-05</v>
       </c>
       <c r="M2" t="str">
-        <v>2026-01-20</v>
+        <v>Dismissed</v>
       </c>
       <c r="N2" t="str">
-        <v>pending</v>
+        <v>Fine of P5000</v>
       </c>
       <c r="O2" t="str">
-        <v>15k</v>
-      </c>
-      <c r="P2" t="str">
-        <v>N/A</v>
+        <v>/uploads/index_cards/indexcard-1769145928098-113952033.png</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3">
-        <v>7</v>
+      <c r="A3" t="str">
+        <v>DKT-2024-002</v>
       </c>
       <c r="B3" t="str">
-        <v>13242141</v>
+        <v>2024-02-16</v>
       </c>
       <c r="C3" t="str">
-        <v>Invalid Date</v>
+        <v>PNP Tagbilaran</v>
       </c>
       <c r="D3" t="str">
-        <v>manny</v>
+        <v>Jane Smith</v>
       </c>
       <c r="E3" t="str">
-        <v>clifford</v>
+        <v>loon</v>
       </c>
       <c r="F3" t="str">
-        <v>San isidro</v>
+        <v>Assault</v>
       </c>
       <c r="G3" t="str">
-        <v>theft</v>
+        <v>Invalid Date</v>
       </c>
       <c r="H3" t="str">
-        <v>Invalid Date</v>
+        <v>2024-04-11</v>
       </c>
       <c r="I3" t="str">
-        <v>2026-01-08</v>
+        <v>Prosecutor Garcia</v>
       </c>
       <c r="J3" t="str">
-        <v>james</v>
+        <v>CRIM-2024-002</v>
       </c>
       <c r="K3" t="str">
-        <v>Reppublic Act 2104</v>
+        <v>Branch 2</v>
       </c>
       <c r="L3" t="str">
-        <v>Tagbi</v>
+        <v>2024-03-11</v>
       </c>
       <c r="M3" t="str">
-        <v>2026-01-09</v>
+        <v>Convicted</v>
       </c>
       <c r="N3" t="str">
-        <v>pending</v>
+        <v>Pending</v>
       </c>
       <c r="O3" t="str">
-        <v>14k</v>
-      </c>
-      <c r="P3" t="str">
-        <v>N/A</v>
+        <v>/uploads/index_cards/indexcard-1769145953585-913133096.png</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4">
-        <v>9</v>
+      <c r="A4" t="str">
+        <v>3232</v>
       </c>
       <c r="B4" t="str">
-        <v>76543232</v>
+        <v>2026-01-06</v>
       </c>
       <c r="C4" t="str">
-        <v>Invalid Date</v>
+        <v>keynn</v>
       </c>
       <c r="D4" t="str">
-        <v>namiiiii</v>
+        <v>trekk</v>
       </c>
       <c r="E4" t="str">
-        <v>chriss</v>
+        <v>San Isidro</v>
       </c>
       <c r="F4" t="str">
-        <v>buol</v>
+        <v>robbery</v>
       </c>
       <c r="G4" t="str">
-        <v>raped</v>
+        <v>Invalid Date</v>
       </c>
       <c r="H4" t="str">
-        <v>Invalid Date</v>
+        <v>2026-01-07</v>
       </c>
       <c r="I4" t="str">
-        <v>2026-01-13</v>
+        <v>Atty.batman</v>
       </c>
       <c r="J4" t="str">
-        <v>Atty. Doroy</v>
+        <v>Reppublic Act 2104</v>
       </c>
       <c r="K4" t="str">
-        <v>N/A</v>
+        <v>Tagbi</v>
       </c>
       <c r="L4" t="str">
-        <v>Capitol</v>
+        <v>2026-01-08</v>
       </c>
       <c r="M4" t="str">
-        <v>2026-01-22</v>
+        <v>Pending</v>
       </c>
       <c r="N4" t="str">
-        <v>pending</v>
+        <v>14k</v>
       </c>
       <c r="O4" t="str">
-        <v>15k</v>
-      </c>
-      <c r="P4" t="str">
-        <v>N/A</v>
+        <v>/uploads/index_cards/indexcard-1769146086538-553986725.png</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5">
-        <v>10</v>
+      <c r="A5" t="str">
+        <v>245232</v>
       </c>
       <c r="B5" t="str">
-        <v>235845323</v>
+        <v>2026-01-05</v>
       </c>
       <c r="C5" t="str">
-        <v>2026-02-06</v>
+        <v>koynnn</v>
       </c>
       <c r="D5" t="str">
-        <v>jek2</v>
+        <v>kart</v>
       </c>
       <c r="E5" t="str">
-        <v>zuma</v>
+        <v xml:space="preserve">Tiptip </v>
       </c>
       <c r="F5" t="str">
-        <v>manalo</v>
+        <v>grave threat</v>
       </c>
       <c r="G5" t="str">
-        <v>grave threat</v>
+        <v>Invalid Date</v>
       </c>
       <c r="H5" t="str">
-        <v>2026-01-29</v>
+        <v>2026-01-28</v>
       </c>
       <c r="I5" t="str">
-        <v>Invalid Date</v>
+        <v>Atty. Superman</v>
       </c>
       <c r="J5" t="str">
-        <v>Atty .spiderman</v>
+        <v>N/A</v>
       </c>
       <c r="K5" t="str">
-        <v>N/A</v>
+        <v>tagbi</v>
       </c>
       <c r="L5" t="str">
-        <v>N/A</v>
+        <v>2026-01-27</v>
       </c>
       <c r="M5" t="str">
-        <v>2026-01-21</v>
+        <v>Dismissed</v>
       </c>
       <c r="N5" t="str">
-        <v>Dismissed</v>
+        <v>12k</v>
       </c>
       <c r="O5" t="str">
-        <v>23k</v>
-      </c>
-      <c r="P5" t="str">
-        <v>N/A</v>
+        <v>/uploads/index_cards/indexcard-1769146194762-537518850.png</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6">
-        <v>11</v>
+      <c r="A6" t="str">
+        <v>4121214</v>
       </c>
       <c r="B6" t="str">
-        <v>16234</v>
+        <v>2026-01-29</v>
       </c>
       <c r="C6" t="str">
-        <v>2026-01-07</v>
+        <v>shaaan</v>
       </c>
       <c r="D6" t="str">
-        <v>roxanne</v>
+        <v>kroel</v>
       </c>
       <c r="E6" t="str">
-        <v>kristtian</v>
+        <v>Dauis</v>
       </c>
       <c r="F6" t="str">
-        <v>cabanugan</v>
+        <v>raped</v>
       </c>
       <c r="G6" t="str">
-        <v>robbery</v>
+        <v>Invalid Date</v>
       </c>
       <c r="H6" t="str">
-        <v>Invalid Date</v>
+        <v>2026-01-13</v>
       </c>
       <c r="I6" t="str">
-        <v>2026-01-08</v>
+        <v>Atty. Doroy</v>
       </c>
       <c r="J6" t="str">
-        <v>james</v>
+        <v>N/A</v>
       </c>
       <c r="K6" t="str">
-        <v>Reppublic Act 2104</v>
+        <v>Capitol</v>
       </c>
       <c r="L6" t="str">
-        <v>Tagbi</v>
+        <v>2026-01-22</v>
       </c>
       <c r="M6" t="str">
-        <v>2026-01-09</v>
+        <v>pending</v>
       </c>
       <c r="N6" t="str">
-        <v>pending</v>
+        <v>15k</v>
       </c>
       <c r="O6" t="str">
-        <v>14k</v>
-      </c>
-      <c r="P6" t="str">
         <v>N/A</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7">
-        <v>12</v>
+      <c r="A7" t="str">
+        <v>13242141</v>
       </c>
       <c r="B7" t="str">
-        <v>72341</v>
+        <v>Invalid Date</v>
       </c>
       <c r="C7" t="str">
-        <v>2026-01-07</v>
+        <v>manny</v>
       </c>
       <c r="D7" t="str">
-        <v>marcilene</v>
+        <v>clifford</v>
       </c>
       <c r="E7" t="str">
-        <v>shielouu</v>
+        <v>San isidro</v>
       </c>
       <c r="F7" t="str">
-        <v>cansage norte</v>
+        <v>theft</v>
       </c>
       <c r="G7" t="str">
-        <v>grave threat</v>
+        <v>Invalid Date</v>
       </c>
       <c r="H7" t="str">
-        <v>Invalid Date</v>
+        <v>2026-01-08</v>
       </c>
       <c r="I7" t="str">
-        <v>2026-01-30</v>
+        <v>james</v>
       </c>
       <c r="J7" t="str">
-        <v>Atty. Superman</v>
+        <v>Reppublic Act 2104</v>
       </c>
       <c r="K7" t="str">
-        <v>N/A</v>
+        <v>Tagbi</v>
       </c>
       <c r="L7" t="str">
-        <v>tagbi</v>
+        <v>2026-01-09</v>
       </c>
       <c r="M7" t="str">
-        <v>2026-01-29</v>
+        <v>pending</v>
       </c>
       <c r="N7" t="str">
-        <v>Convicted</v>
+        <v>14k</v>
       </c>
       <c r="O7" t="str">
-        <v>100k</v>
-      </c>
-      <c r="P7" t="str">
         <v>N/A</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8">
-        <v>13</v>
+      <c r="A8" t="str">
+        <v>65243242</v>
       </c>
       <c r="B8" t="str">
-        <v>115532</v>
+        <v>Invalid Date</v>
       </c>
       <c r="C8" t="str">
-        <v>2026-01-29</v>
+        <v>emann</v>
       </c>
       <c r="D8" t="str">
-        <v>mercyyy</v>
+        <v>clifff</v>
       </c>
       <c r="E8" t="str">
-        <v>tibinn</v>
+        <v>maribojoc</v>
       </c>
       <c r="F8" t="str">
-        <v>baunos</v>
+        <v xml:space="preserve">tax </v>
       </c>
       <c r="G8" t="str">
-        <v>raped</v>
+        <v>Invalid Date</v>
       </c>
       <c r="H8" t="str">
-        <v>Invalid Date</v>
+        <v>2026-01-25</v>
       </c>
       <c r="I8" t="str">
-        <v>2026-01-13</v>
+        <v>Atty. Superman</v>
       </c>
       <c r="J8" t="str">
-        <v>Atty. Doroy</v>
+        <v>N/A</v>
       </c>
       <c r="K8" t="str">
-        <v>N/A</v>
+        <v>tagbi</v>
       </c>
       <c r="L8" t="str">
-        <v>Capitol</v>
+        <v>2026-01-24</v>
       </c>
       <c r="M8" t="str">
-        <v>2026-01-22</v>
+        <v>Convicted</v>
       </c>
       <c r="N8" t="str">
-        <v>Dismissed</v>
+        <v>12k</v>
       </c>
       <c r="O8" t="str">
-        <v>190k</v>
-      </c>
-      <c r="P8" t="str">
         <v>N/A</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9">
-        <v>14</v>
+      <c r="A9" t="str">
+        <v>76543232</v>
       </c>
       <c r="B9" t="str">
-        <v>3232</v>
+        <v>Invalid Date</v>
       </c>
       <c r="C9" t="str">
-        <v>2026-01-07</v>
+        <v>namiiiii</v>
       </c>
       <c r="D9" t="str">
-        <v>keynn</v>
+        <v>chriss</v>
       </c>
       <c r="E9" t="str">
-        <v>trekk</v>
+        <v>buol</v>
       </c>
       <c r="F9" t="str">
-        <v>San Isidro</v>
+        <v>raped</v>
       </c>
       <c r="G9" t="str">
-        <v>robbery</v>
+        <v>Invalid Date</v>
       </c>
       <c r="H9" t="str">
-        <v>Invalid Date</v>
+        <v>2026-01-13</v>
       </c>
       <c r="I9" t="str">
-        <v>2026-01-08</v>
+        <v>Atty. Doroy</v>
       </c>
       <c r="J9" t="str">
-        <v>Atty.batman</v>
+        <v>N/A</v>
       </c>
       <c r="K9" t="str">
-        <v>Reppublic Act 2104</v>
+        <v>Capitol</v>
       </c>
       <c r="L9" t="str">
-        <v>Tagbi</v>
+        <v>2026-01-22</v>
       </c>
       <c r="M9" t="str">
-        <v>2026-01-09</v>
+        <v>pending</v>
       </c>
       <c r="N9" t="str">
-        <v>pending</v>
+        <v>15k</v>
       </c>
       <c r="O9" t="str">
-        <v>14k</v>
-      </c>
-      <c r="P9" t="str">
-        <v>N/A</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10">
-        <v>15</v>
-      </c>
-      <c r="B10" t="str">
-        <v>245232</v>
-      </c>
-      <c r="C10" t="str">
-        <v>2026-01-07</v>
-      </c>
-      <c r="D10" t="str">
-        <v>koynnn</v>
-      </c>
-      <c r="E10" t="str">
-        <v>kart</v>
-      </c>
-      <c r="F10" t="str">
-        <v xml:space="preserve">Tiptip </v>
-      </c>
-      <c r="G10" t="str">
-        <v>grave threat</v>
-      </c>
-      <c r="H10" t="str">
-        <v>Invalid Date</v>
-      </c>
-      <c r="I10" t="str">
-        <v>2026-01-30</v>
-      </c>
-      <c r="J10" t="str">
-        <v>Atty. Superman</v>
-      </c>
-      <c r="K10" t="str">
-        <v>N/A</v>
-      </c>
-      <c r="L10" t="str">
-        <v>tagbi</v>
-      </c>
-      <c r="M10" t="str">
-        <v>2026-01-29</v>
-      </c>
-      <c r="N10" t="str">
-        <v>terminated</v>
-      </c>
-      <c r="O10" t="str">
-        <v>12k</v>
-      </c>
-      <c r="P10" t="str">
-        <v>N/A</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11">
-        <v>16</v>
-      </c>
-      <c r="B11" t="str">
-        <v>4121214</v>
-      </c>
-      <c r="C11" t="str">
-        <v>2026-01-29</v>
-      </c>
-      <c r="D11" t="str">
-        <v>shaaan</v>
-      </c>
-      <c r="E11" t="str">
-        <v>kroel</v>
-      </c>
-      <c r="F11" t="str">
-        <v>Dauis</v>
-      </c>
-      <c r="G11" t="str">
-        <v>raped</v>
-      </c>
-      <c r="H11" t="str">
-        <v>Invalid Date</v>
-      </c>
-      <c r="I11" t="str">
-        <v>2026-01-13</v>
-      </c>
-      <c r="J11" t="str">
-        <v>Atty. Doroy</v>
-      </c>
-      <c r="K11" t="str">
-        <v>N/A</v>
-      </c>
-      <c r="L11" t="str">
-        <v>Capitol</v>
-      </c>
-      <c r="M11" t="str">
-        <v>2026-01-22</v>
-      </c>
-      <c r="N11" t="str">
-        <v>pending</v>
-      </c>
-      <c r="O11" t="str">
-        <v>15k</v>
-      </c>
-      <c r="P11" t="str">
         <v>N/A</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:P11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:O9"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>